<commit_message>
update TCs & RTM
</commit_message>
<xml_diff>
--- a/Monitor and Control/Traceability Matrix .xlsx
+++ b/Monitor and Control/Traceability Matrix .xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61BE18C-4D5E-4849-8321-5BE358167029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3AC9AE-C514-4C87-B36F-645C8AED3C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,10 +586,6 @@
 TC_AddTour_026</t>
   </si>
   <si>
-    <t>TC_Thank_You_001
-TC_Thank_You_002</t>
-  </si>
-  <si>
     <t>TC_User_Sign_Up_001</t>
   </si>
   <si>
@@ -627,13 +623,20 @@
     <t>TC_User_Sign_Up_018</t>
   </si>
   <si>
-    <t>TC_User_Home_001</t>
-  </si>
-  <si>
-    <t>TC_User_Book_001</t>
-  </si>
-  <si>
     <t>TC_AddTour_001</t>
+  </si>
+  <si>
+    <t>TC_User_Home_001
+TC_User_Book_001</t>
+  </si>
+  <si>
+    <t>TC_User_Book_003</t>
+  </si>
+  <si>
+    <t>TC_User_Book_002
+TC_User_Book_004
+TC_Thank_You_001
+TC_Thank_You_002</t>
   </si>
 </sst>
 </file>
@@ -644,13 +647,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1154,18 +1157,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="D23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="1" max="2" width="40.69921875" customWidth="1"/>
+    <col min="3" max="3" width="40.8984375" customWidth="1"/>
     <col min="4" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.09765625" customWidth="1"/>
+    <col min="7" max="7" width="35.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,7 +1209,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>112</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,10 +1248,10 @@
         <v>96</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -1261,10 +1264,10 @@
         <v>96</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -1277,10 +1280,10 @@
         <v>96</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1293,10 +1296,10 @@
         <v>96</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -1309,10 +1312,10 @@
         <v>96</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -1325,7 +1328,7 @@
         <v>96</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1341,7 +1344,7 @@
         <v>96</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1357,7 +1360,7 @@
         <v>96</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1373,7 +1376,7 @@
         <v>111</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,7 +1633,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>30</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>121</v>
       </c>
@@ -1694,11 +1697,11 @@
       <c r="G32" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="C33" s="26"/>
@@ -1713,7 +1716,7 @@
         <v>106</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1760,7 +1763,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -1776,7 +1779,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -1792,7 +1795,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -1824,7 +1827,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="69" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -1840,7 +1843,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -2209,10 +2212,10 @@
         <v>119</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="69" x14ac:dyDescent="0.25">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="20"/>
@@ -2228,7 +2231,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A66" s="20"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20"/>
@@ -2244,7 +2247,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="138" x14ac:dyDescent="0.25">
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="C67" s="20"/>
@@ -2276,7 +2279,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A69" s="20"/>
       <c r="B69" s="20"/>
       <c r="C69" s="20"/>
@@ -2292,7 +2295,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
@@ -2308,7 +2311,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
addin bug colum to the RTM
</commit_message>
<xml_diff>
--- a/Monitor and Control/Traceability Matrix .xlsx
+++ b/Monitor and Control/Traceability Matrix .xlsx
@@ -5,27 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3AC9AE-C514-4C87-B36F-645C8AED3C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB45CE4D-9B3F-4D9D-8BFC-68E94795C1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="195">
   <si>
     <t>Specific requirements</t>
   </si>
@@ -626,17 +636,44 @@
     <t>TC_AddTour_001</t>
   </si>
   <si>
-    <t>TC_User_Home_001
-TC_User_Book_001</t>
-  </si>
-  <si>
     <t>TC_User_Book_003</t>
   </si>
   <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>LoginUser_001</t>
+  </si>
+  <si>
+    <t>LoginUser_002</t>
+  </si>
+  <si>
+    <t>LoginUser_003</t>
+  </si>
+  <si>
+    <t>LoginUser_004</t>
+  </si>
+  <si>
+    <t>LoginUser_005</t>
+  </si>
+  <si>
+    <t>LoginUser_006</t>
+  </si>
+  <si>
+    <t>LoginUser_007</t>
+  </si>
+  <si>
+    <t>LoginUser_008</t>
+  </si>
+  <si>
+    <t>AdminHome_001</t>
+  </si>
+  <si>
+    <t>TC_User_Home_001</t>
+  </si>
+  <si>
     <t>TC_User_Book_002
-TC_User_Book_004
-TC_Thank_You_001
-TC_Thank_You_002</t>
+TC_User_Book_004</t>
   </si>
 </sst>
 </file>
@@ -647,13 +684,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -783,15 +820,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,10 +858,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,19 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -863,16 +885,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1155,231 +1189,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H146"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="40.69921875" customWidth="1"/>
-    <col min="3" max="3" width="40.8984375" customWidth="1"/>
+    <col min="1" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
     <col min="4" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="32.09765625" customWidth="1"/>
-    <col min="7" max="7" width="35.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.69921875" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="31" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="6" t="s">
+      <c r="I1" s="31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="7" t="s">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="7" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="7" t="s">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="7" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="7" t="s">
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="7" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="7" t="s">
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="7" t="s">
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="7" t="s">
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="7" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="7" t="s">
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="7" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="14" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="7" t="s">
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="7" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="7" t="s">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="7" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="7" t="s">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="7" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>29</v>
       </c>
@@ -1389,7 +1437,7 @@
       <c r="C13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="16" t="s">
@@ -1398,294 +1446,347 @@
       <c r="F13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="17"/>
+      <c r="I13" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="11" t="s">
+      <c r="I14" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="10" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="11" t="s">
+      <c r="I15" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="11" t="s">
+      <c r="I16" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="10" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="11" t="s">
+      <c r="I17" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="10" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="17"/>
+      <c r="I18" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="11" t="s">
+      <c r="I19" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="10" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="8" t="s">
+      <c r="I20" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="8" t="s">
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="10" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="10" t="s">
+      <c r="I21" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="8" t="s">
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="8" t="s">
+      <c r="I22" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="11" t="s">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="10" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="17"/>
+      <c r="I23" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
       <c r="G24" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="10" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="11" t="s">
+      <c r="I24" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="10" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="17"/>
+      <c r="I25" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="21"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="13" t="s">
+      <c r="I26" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="21"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="12" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="11" t="s">
+      <c r="I27" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="11" t="s">
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="10" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="11" t="s">
+      <c r="I28" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="11" t="s">
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="I29" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="14" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="7" t="s">
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="7" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="6" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>121</v>
       </c>
       <c r="B32" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -1694,50 +1795,53 @@
       <c r="F32" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="8" t="s">
+      <c r="H32" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="8" t="s">
+      <c r="F33" s="21"/>
+      <c r="G33" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="8" t="s">
+      <c r="H33" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="8" t="s">
+      <c r="F34" s="17"/>
+      <c r="G34" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H34" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="I34" s="15"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>125</v>
       </c>
@@ -1747,7 +1851,7 @@
       <c r="C35" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E35" s="16" t="s">
@@ -1756,276 +1860,294 @@
       <c r="F35" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="7" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="8" t="s">
+      <c r="I35" s="15"/>
+    </row>
+    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="8" t="s">
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="8" t="s">
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="8" t="s">
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="8" t="s">
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="8" t="s">
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="8" t="s">
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="8" t="s">
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="12" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="69" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="8" t="s">
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="8" t="s">
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" s="12" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="8" t="s">
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="8" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" s="12" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="8" t="s">
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="8" t="s">
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="I42" s="15"/>
+    </row>
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F43" s="19" t="s">
+      <c r="F43" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="7" t="s">
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="19"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="7" t="s">
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="7" t="s">
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="19"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="7" t="s">
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="7" t="s">
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="7" t="s">
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="7" t="s">
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="7" t="s">
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="7" t="s">
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="19"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="7" t="s">
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="7" t="s">
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="19"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="7" t="s">
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="7" t="s">
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="19"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="7" t="s">
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="7" t="s">
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="7" t="s">
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="7" t="s">
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="20"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="7" t="s">
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
         <v>42</v>
       </c>
@@ -2035,7 +2157,7 @@
       <c r="C53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="7" t="s">
         <v>54</v>
       </c>
       <c r="E53" s="16" t="s">
@@ -2044,274 +2166,292 @@
       <c r="F53" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H53" s="8"/>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="8" t="s">
+      <c r="H53" s="7"/>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="8" t="s">
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H54" s="8"/>
-    </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="8" t="s">
+      <c r="H54" s="7"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="8" t="s">
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H55" s="8"/>
-    </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="8" t="s">
+      <c r="H55" s="7"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="8" t="s">
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="8" t="s">
+      <c r="H56" s="7"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="8" t="s">
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H57" s="8"/>
-    </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="8" t="s">
+      <c r="H57" s="7"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="8" t="s">
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H58" s="8"/>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="8" t="s">
+      <c r="H58" s="7"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="8" t="s">
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H59" s="8"/>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="8" t="s">
+      <c r="H59" s="7"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="8" t="s">
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H60" s="8"/>
-    </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="8" t="s">
+      <c r="H60" s="7"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="8" t="s">
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H61" s="8"/>
-    </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="8" t="s">
+      <c r="H61" s="7"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="8" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="H62" s="8"/>
-    </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="8" t="s">
+      <c r="H62" s="7"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="8" t="s">
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H63" s="8"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="H63" s="7"/>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F64" s="19" t="s">
+      <c r="F64" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G64" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H64" s="6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="69" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="7" t="s">
+      <c r="I64" s="6"/>
+    </row>
+    <row r="65" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="7" t="s">
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H65" s="15" t="s">
+      <c r="H65" s="14" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="7" t="s">
+      <c r="I65" s="14"/>
+    </row>
+    <row r="66" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="7" t="s">
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H66" s="15" t="s">
+      <c r="H66" s="14" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="138" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="7" t="s">
+      <c r="I66" s="14"/>
+    </row>
+    <row r="67" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="7" t="s">
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H67" s="15" t="s">
+      <c r="H67" s="14" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="7" t="s">
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="7" t="s">
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="H68" s="6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="7" t="s">
+      <c r="I68" s="6"/>
+    </row>
+    <row r="69" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="7" t="s">
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H69" s="15" t="s">
+      <c r="H69" s="14" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="7" t="s">
+      <c r="I69" s="14"/>
+    </row>
+    <row r="70" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="7" t="s">
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="H70" s="15" t="s">
+      <c r="H70" s="14" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="14"/>
+    </row>
+    <row r="71" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>126</v>
       </c>
@@ -2321,7 +2461,7 @@
       <c r="C71" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E71" s="16" t="s">
@@ -2333,77 +2473,93 @@
       <c r="G71" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="9" t="s">
+      <c r="I71" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
       <c r="H72" s="16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="11" t="s">
+      <c r="I72" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="18"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
       <c r="D74" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="11" t="s">
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="10" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="11" t="s">
+      <c r="I74" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="11" t="s">
+      <c r="I75" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="17"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="11" t="s">
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="10" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2412,8 +2568,9 @@
       <c r="F77" s="3"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2422,8 +2579,9 @@
       <c r="F78" s="3"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2432,8 +2590,9 @@
       <c r="F79" s="3"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2442,8 +2601,9 @@
       <c r="F80" s="3"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2452,8 +2612,9 @@
       <c r="F81" s="3"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2462,8 +2623,9 @@
       <c r="F82" s="3"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2472,8 +2634,9 @@
       <c r="F83" s="3"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2482,8 +2645,9 @@
       <c r="F84" s="3"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2492,8 +2656,9 @@
       <c r="F85" s="3"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2502,8 +2667,9 @@
       <c r="F86" s="3"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2512,8 +2678,9 @@
       <c r="F87" s="3"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2522,8 +2689,9 @@
       <c r="F88" s="3"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2532,8 +2700,9 @@
       <c r="F89" s="3"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2542,8 +2711,9 @@
       <c r="F90" s="3"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2552,8 +2722,9 @@
       <c r="F91" s="3"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2562,8 +2733,9 @@
       <c r="F92" s="3"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2572,8 +2744,9 @@
       <c r="F93" s="3"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2582,8 +2755,9 @@
       <c r="F94" s="3"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2592,8 +2766,9 @@
       <c r="F95" s="3"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2602,8 +2777,9 @@
       <c r="F96" s="3"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2612,8 +2788,9 @@
       <c r="F97" s="3"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2622,8 +2799,9 @@
       <c r="F98" s="3"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2632,8 +2810,9 @@
       <c r="F99" s="3"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2642,8 +2821,9 @@
       <c r="F100" s="3"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2652,8 +2832,9 @@
       <c r="F101" s="3"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2662,8 +2843,9 @@
       <c r="F102" s="3"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2672,8 +2854,9 @@
       <c r="F103" s="3"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2682,8 +2865,9 @@
       <c r="F104" s="3"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2692,8 +2876,9 @@
       <c r="F105" s="3"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2702,8 +2887,9 @@
       <c r="F106" s="3"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2712,8 +2898,9 @@
       <c r="F107" s="3"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2722,8 +2909,9 @@
       <c r="F108" s="3"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2732,8 +2920,9 @@
       <c r="F109" s="3"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2742,8 +2931,9 @@
       <c r="F110" s="3"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2752,8 +2942,9 @@
       <c r="F111" s="3"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2762,8 +2953,9 @@
       <c r="F112" s="3"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2772,8 +2964,9 @@
       <c r="F113" s="3"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="1"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2782,8 +2975,9 @@
       <c r="F114" s="3"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2792,8 +2986,9 @@
       <c r="F115" s="3"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2802,8 +2997,9 @@
       <c r="F116" s="3"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2812,8 +3008,9 @@
       <c r="F117" s="3"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2822,8 +3019,9 @@
       <c r="F118" s="3"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2832,8 +3030,9 @@
       <c r="F119" s="3"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2842,8 +3041,9 @@
       <c r="F120" s="3"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2852,8 +3052,9 @@
       <c r="F121" s="3"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2862,8 +3063,9 @@
       <c r="F122" s="3"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2872,8 +3074,9 @@
       <c r="F123" s="3"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2882,8 +3085,9 @@
       <c r="F124" s="3"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2892,8 +3096,9 @@
       <c r="F125" s="3"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2902,8 +3107,9 @@
       <c r="F126" s="3"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2912,8 +3118,9 @@
       <c r="F127" s="3"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2922,8 +3129,9 @@
       <c r="F128" s="3"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="1"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -2932,8 +3140,9 @@
       <c r="F129" s="3"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="1"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -2942,8 +3151,9 @@
       <c r="F130" s="3"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -2952,8 +3162,9 @@
       <c r="F131" s="3"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -2962,8 +3173,9 @@
       <c r="F132" s="3"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -2972,8 +3184,9 @@
       <c r="F133" s="3"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -2982,8 +3195,9 @@
       <c r="F134" s="3"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -2992,8 +3206,9 @@
       <c r="F135" s="3"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="1"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3002,8 +3217,9 @@
       <c r="F136" s="3"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="1"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3012,8 +3228,9 @@
       <c r="F137" s="3"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="1"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3022,8 +3239,9 @@
       <c r="F138" s="3"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="1"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3032,8 +3250,9 @@
       <c r="F139" s="3"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="1"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3042,8 +3261,9 @@
       <c r="F140" s="3"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="1"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3052,8 +3272,9 @@
       <c r="F141" s="3"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="1"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3062,8 +3283,9 @@
       <c r="F142" s="3"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="1"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3072,8 +3294,9 @@
       <c r="F143" s="3"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="1"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3082,8 +3305,9 @@
       <c r="F144" s="3"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="1"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3092,8 +3316,9 @@
       <c r="F145" s="3"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="1"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3102,9 +3327,61 @@
       <c r="F146" s="3"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="64">
+    <mergeCell ref="I72:I73"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="C64:C70"/>
+    <mergeCell ref="A64:A70"/>
+    <mergeCell ref="B43:B52"/>
+    <mergeCell ref="B64:B70"/>
+    <mergeCell ref="C43:C52"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C53:C63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B53:B63"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="E35:E42"/>
+    <mergeCell ref="F35:F42"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="C35:C42"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="F64:F70"/>
+    <mergeCell ref="E43:E52"/>
+    <mergeCell ref="E64:E70"/>
+    <mergeCell ref="E53:E63"/>
+    <mergeCell ref="F53:F63"/>
+    <mergeCell ref="F43:F52"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="A13:A29"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C13:C29"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="H72:H73"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E71:E76"/>
+    <mergeCell ref="F71:F76"/>
+    <mergeCell ref="G71:G76"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="G26:G27"/>
@@ -3118,53 +3395,6 @@
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="F3:F12"/>
-    <mergeCell ref="H72:H73"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E71:E76"/>
-    <mergeCell ref="F71:F76"/>
-    <mergeCell ref="G71:G76"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C13:C29"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="A13:A29"/>
-    <mergeCell ref="B13:B29"/>
-    <mergeCell ref="F64:F70"/>
-    <mergeCell ref="E43:E52"/>
-    <mergeCell ref="E64:E70"/>
-    <mergeCell ref="E53:E63"/>
-    <mergeCell ref="F53:F63"/>
-    <mergeCell ref="F43:F52"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="E35:E42"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="C35:C42"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B43:B52"/>
-    <mergeCell ref="B64:B70"/>
-    <mergeCell ref="C43:C52"/>
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="C53:C63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B53:B63"/>
-    <mergeCell ref="C71:C75"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="C64:C70"/>
-    <mergeCell ref="A64:A70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update RTM adding Bugs
</commit_message>
<xml_diff>
--- a/Monitor and Control/Traceability Matrix .xlsx
+++ b/Monitor and Control/Traceability Matrix .xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\Travel_Advisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8832525E-B343-4BDC-9933-F9F02AE71E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E812D6B-B5D5-4428-8649-826D963D1261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="211">
   <si>
     <t>Specific requirements</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>Layout_Tour</t>
-  </si>
-  <si>
-    <t>Layout_Tour &amp; Layout_Thank_you</t>
   </si>
   <si>
     <t>Layout_Add_Admin</t>
@@ -598,9 +595,6 @@
     <t>TC_User_Sign_Up_018</t>
   </si>
   <si>
-    <t>TC_AddTour_001</t>
-  </si>
-  <si>
     <t>Bugs</t>
   </si>
   <si>
@@ -688,6 +682,45 @@
   </si>
   <si>
     <t>User_Sign_Up_002</t>
+  </si>
+  <si>
+    <t>TC_AddTour_027,TC_AddTour_028</t>
+  </si>
+  <si>
+    <t>AddTour_001</t>
+  </si>
+  <si>
+    <t>Customer_Reqirement_08</t>
+  </si>
+  <si>
+    <t>User navigate to thank you page after login</t>
+  </si>
+  <si>
+    <t>REQ-01-ThankYou</t>
+  </si>
+  <si>
+    <t>REQ-02-ThankYou</t>
+  </si>
+  <si>
+    <t>REQ-03-ThankYou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layout_Tour </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Layout_Thank_you</t>
+  </si>
+  <si>
+    <t>TC_Thank_You_001</t>
+  </si>
+  <si>
+    <t>TC_Thank_You_002</t>
+  </si>
+  <si>
+    <t>TC_Thank_You_003</t>
+  </si>
+  <si>
+    <t>ThankYouLayout.aspx</t>
   </si>
 </sst>
 </file>
@@ -698,13 +731,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1205,18 +1238,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78:G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="40.69921875" customWidth="1"/>
-    <col min="3" max="3" width="40.8984375" customWidth="1"/>
+    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
     <col min="4" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="32.09765625" customWidth="1"/>
-    <col min="7" max="7" width="35.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="29.69921875" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1224,7 +1257,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>27</v>
@@ -1243,10 +1276,10 @@
         <v>3</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -1266,7 +1299,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>74</v>
@@ -1278,16 +1311,16 @@
         <v>75</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,16 +1333,16 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1319,13 +1352,13 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1338,16 +1371,16 @@
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -1357,13 +1390,13 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1376,16 +1409,16 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="58.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -1395,16 +1428,16 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1414,16 +1447,16 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -1433,13 +1466,13 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,13 +1485,13 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1466,7 +1499,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>4</v>
@@ -1478,16 +1511,16 @@
         <v>76</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1500,13 +1533,13 @@
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1518,10 +1551,10 @@
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
       <c r="H15" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1533,10 +1566,10 @@
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1548,10 +1581,10 @@
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="H17" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1563,10 +1596,10 @@
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1579,13 +1612,13 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1597,10 +1630,10 @@
       <c r="F20" s="22"/>
       <c r="G20" s="23"/>
       <c r="H20" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1613,13 +1646,13 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
       <c r="G21" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1632,13 +1665,13 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1651,13 +1684,13 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1670,13 +1703,13 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,10 +1721,10 @@
       <c r="F25" s="22"/>
       <c r="G25" s="23"/>
       <c r="H25" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1699,18 +1732,18 @@
       <c r="B26" s="28"/>
       <c r="C26" s="22"/>
       <c r="D26" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1722,10 +1755,10 @@
       <c r="F27" s="22"/>
       <c r="G27" s="23"/>
       <c r="H27" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1733,18 +1766,18 @@
       <c r="B28" s="28"/>
       <c r="C28" s="22"/>
       <c r="D28" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1752,44 +1785,44 @@
       <c r="B29" s="29"/>
       <c r="C29" s="23"/>
       <c r="D29" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
       <c r="G29" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I30" s="14"/>
     </row>
@@ -1798,27 +1831,27 @@
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="C32" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>23</v>
@@ -1827,19 +1860,19 @@
         <v>77</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="28"/>
       <c r="C33" s="22"/>
@@ -1847,15 +1880,15 @@
         <v>24</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>78</v>
+        <v>205</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1871,10 +1904,10 @@
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
       <c r="H34" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1882,24 +1915,24 @@
       <c r="B35" s="29"/>
       <c r="C35" s="23"/>
       <c r="D35" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>32</v>
@@ -1911,17 +1944,17 @@
         <v>76</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I36" s="15"/>
     </row>
-    <row r="37" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -1931,14 +1964,14 @@
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -1948,14 +1981,14 @@
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
       <c r="G38" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -1965,10 +1998,10 @@
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
       <c r="G39" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I39" s="12"/>
     </row>
@@ -1982,14 +2015,14 @@
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
       <c r="G40" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I40" s="12"/>
     </row>
-    <row r="41" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
@@ -1999,14 +2032,14 @@
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
       <c r="G41" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I41" s="12"/>
     </row>
-    <row r="42" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
@@ -2016,10 +2049,10 @@
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
       <c r="G42" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I42" s="12"/>
     </row>
@@ -2033,10 +2066,10 @@
       <c r="E43" s="23"/>
       <c r="F43" s="23"/>
       <c r="G43" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I43" s="15"/>
     </row>
@@ -2045,7 +2078,7 @@
         <v>31</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>41</v>
@@ -2054,13 +2087,13 @@
         <v>43</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -2075,7 +2108,7 @@
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
       <c r="G45" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -2090,7 +2123,7 @@
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -2105,7 +2138,7 @@
       <c r="E47" s="19"/>
       <c r="F47" s="19"/>
       <c r="G47" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -2120,7 +2153,7 @@
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -2135,7 +2168,7 @@
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
       <c r="G49" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -2150,7 +2183,7 @@
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
       <c r="G50" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -2165,7 +2198,7 @@
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
       <c r="G51" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -2180,7 +2213,7 @@
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
       <c r="G52" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -2195,7 +2228,7 @@
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
       <c r="G53" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -2205,7 +2238,7 @@
         <v>42</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>53</v>
@@ -2214,13 +2247,13 @@
         <v>54</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="15"/>
@@ -2235,7 +2268,7 @@
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
       <c r="G55" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="15"/>
@@ -2250,7 +2283,7 @@
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
       <c r="G56" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="15"/>
@@ -2265,7 +2298,7 @@
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
       <c r="G57" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="15"/>
@@ -2280,7 +2313,7 @@
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
       <c r="G58" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="15"/>
@@ -2295,7 +2328,7 @@
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
       <c r="G59" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H59" s="7"/>
       <c r="I59" s="15"/>
@@ -2310,7 +2343,7 @@
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
       <c r="G60" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="15"/>
@@ -2325,7 +2358,7 @@
       <c r="E61" s="22"/>
       <c r="F61" s="22"/>
       <c r="G61" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="15"/>
@@ -2340,7 +2373,7 @@
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
       <c r="G62" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="15"/>
@@ -2355,7 +2388,7 @@
       <c r="E63" s="22"/>
       <c r="F63" s="22"/>
       <c r="G63" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="15"/>
@@ -2365,12 +2398,12 @@
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
       <c r="D64" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E64" s="23"/>
       <c r="F64" s="23"/>
       <c r="G64" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H64" s="7"/>
       <c r="I64" s="15"/>
@@ -2380,7 +2413,7 @@
         <v>31</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>64</v>
@@ -2389,20 +2422,22 @@
         <v>65</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="I65" s="6"/>
-    </row>
-    <row r="66" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
@@ -2412,14 +2447,16 @@
       <c r="E66" s="19"/>
       <c r="F66" s="19"/>
       <c r="G66" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="I66" s="14"/>
-    </row>
-    <row r="67" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>
@@ -2429,14 +2466,16 @@
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
       <c r="G67" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="I67" s="14"/>
-    </row>
-    <row r="68" spans="1:9" ht="138" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
@@ -2446,12 +2485,14 @@
       <c r="E68" s="19"/>
       <c r="F68" s="19"/>
       <c r="G68" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="I68" s="14"/>
+        <v>165</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
@@ -2463,14 +2504,16 @@
       <c r="E69" s="19"/>
       <c r="F69" s="19"/>
       <c r="G69" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="19"/>
       <c r="C70" s="19"/>
@@ -2480,14 +2523,16 @@
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
       <c r="G70" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="I70" s="14"/>
-    </row>
-    <row r="71" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="20"/>
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
@@ -2497,40 +2542,42 @@
       <c r="E71" s="20"/>
       <c r="F71" s="20"/>
       <c r="G71" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="I71" s="14"/>
-    </row>
-    <row r="72" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C72" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E72" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G72" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="F72" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G72" s="21" t="s">
-        <v>103</v>
-      </c>
       <c r="H72" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2538,16 +2585,16 @@
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E73" s="22"/>
       <c r="F73" s="22"/>
       <c r="G73" s="22"/>
       <c r="H73" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I73" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2555,7 +2602,7 @@
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="22"/>
@@ -2568,16 +2615,16 @@
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
       <c r="D75" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E75" s="22"/>
       <c r="F75" s="22"/>
       <c r="G75" s="22"/>
       <c r="H75" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2589,10 +2636,10 @@
       <c r="F76" s="22"/>
       <c r="G76" s="22"/>
       <c r="H76" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I76" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2600,83 +2647,113 @@
       <c r="B77" s="23"/>
       <c r="C77" s="11"/>
       <c r="D77" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E77" s="23"/>
       <c r="F77" s="23"/>
       <c r="G77" s="23"/>
       <c r="H77" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I77" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
+      <c r="A78" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E78" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G78" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="H78" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I78" s="16" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="I79" s="21" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
+      <c r="A80" s="22"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="I81" s="16" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
+      <c r="A83" s="23"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
@@ -3383,7 +3460,16 @@
       <c r="I147" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="75">
+    <mergeCell ref="E78:E83"/>
+    <mergeCell ref="F78:F83"/>
+    <mergeCell ref="G78:G83"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="A78:A83"/>
+    <mergeCell ref="B78:B83"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="D81:D82"/>
     <mergeCell ref="I73:I74"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -3399,6 +3485,7 @@
     <mergeCell ref="F54:F64"/>
     <mergeCell ref="F44:F53"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C12"/>
     <mergeCell ref="A72:A77"/>
     <mergeCell ref="B72:B77"/>
     <mergeCell ref="C65:C71"/>
@@ -3416,6 +3503,7 @@
     <mergeCell ref="C36:C43"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A32:A35"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B30:B31"/>
@@ -3424,8 +3512,6 @@
     <mergeCell ref="B3:B12"/>
     <mergeCell ref="A13:A29"/>
     <mergeCell ref="B13:B29"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C13:C29"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="H73:H74"/>

</xml_diff>